<commit_message>
Tämän viikon työt seurantalomakkeeseen
</commit_message>
<xml_diff>
--- a/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
+++ b/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larty\gitrepo\ClassicCarChain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larty\gitrepo\ClassicCarChain\Dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="30">
   <si>
     <t>Viikko</t>
   </si>
@@ -105,7 +105,10 @@
     <t>Jos haluat pysyä aikataulussa, joudut työskentelmään näin monta tuntia viikossa:</t>
   </si>
   <si>
-    <t>Ethereum/geth -harjoituksia. Testiverkon pystytys. Versionhallinnan käyttöönotto.</t>
+    <t>Solidity -harjoituksia.</t>
+  </si>
+  <si>
+    <t>Solidity -harjoituksia. Testiverkon pystytys. Versionhallinnan käyttöönotto.</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +832,7 @@
       </c>
       <c r="J7" s="46">
         <f>SUM(D:D)</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18"/>
     </row>
@@ -895,7 +898,7 @@
       </c>
       <c r="J11" s="49">
         <f ca="1">((J5-J7)/_xlfn.DAYS(J9, NOW())) *7</f>
-        <v>8.5217391304347831</v>
+        <v>8.5477386934673376</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -1287,7 +1290,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F37" s="20"/>
       <c r="I37" s="7"/>
@@ -1367,8 +1370,12 @@
       <c r="C43" s="28">
         <v>42654</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="20"/>
+      <c r="D43" s="17">
+        <v>5</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="F43" s="20"/>
       <c r="I43" s="7"/>
     </row>
@@ -1393,8 +1400,12 @@
       <c r="C45" s="28">
         <v>42656</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="20"/>
+      <c r="D45" s="17">
+        <v>4</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="F45" s="20"/>
       <c r="I45" s="7"/>
     </row>

</xml_diff>

<commit_message>
Tämän viikon työtunnit versionhallintaan
</commit_message>
<xml_diff>
--- a/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
+++ b/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="31">
   <si>
     <t>Viikko</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Solidity -harjoituksia. Testiverkon pystytys. Versionhallinnan käyttöönotto.</t>
+  </si>
+  <si>
+    <t>Meteor-harjoituksia</t>
   </si>
 </sst>
 </file>
@@ -264,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -402,6 +405,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,8 +794,9 @@
     <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="36" style="6" customWidth="1"/>
     <col min="6" max="6" width="37" style="6" customWidth="1"/>
-    <col min="9" max="9" width="37.625" customWidth="1"/>
-    <col min="10" max="10" width="19.875" customWidth="1"/>
+    <col min="8" max="8" width="32.875" customWidth="1"/>
+    <col min="9" max="9" width="10.25" customWidth="1"/>
+    <col min="10" max="10" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -793,112 +824,121 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
-      <c r="I5" s="47" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="46">
+      <c r="I5" s="46">
         <f>27*10</f>
         <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>36</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="54">
         <v>42618</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
-      <c r="I7" s="30" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="46">
+      <c r="I7" s="46">
         <f>SUM(D:D)</f>
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="58">
         <v>42619</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="56"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="58">
         <v>42620</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
-      <c r="I9" s="12" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="28">
+      <c r="I9" s="28">
         <v>42855</v>
       </c>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="58">
         <v>42621</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="58">
         <v>42622</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-      <c r="I11" s="6" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="49">
-        <f ca="1">((J5-J7)/_xlfn.DAYS(J9, NOW())) *7</f>
-        <v>8.5477386934673376</v>
+      <c r="I11" s="49">
+        <f ca="1">((I5-I7)/_xlfn.DAYS(I9, NOW())) *7</f>
+        <v>8.8817204301075261</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -1581,8 +1621,12 @@
       <c r="C58" s="28">
         <v>42669</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="20"/>
+      <c r="D58" s="17">
+        <v>7</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="F58" s="20"/>
       <c r="I58" s="7"/>
     </row>

</xml_diff>

<commit_message>
Tulee vaan virheilmoitus. Veikkaan, että ABI on väärin.
</commit_message>
<xml_diff>
--- a/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
+++ b/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="34">
   <si>
     <t>Viikko</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Meteor-harjoituksia, johdannon kirjoittelua</t>
+  </si>
+  <si>
+    <t>Funktiokutsu sopimuksesta</t>
   </si>
 </sst>
 </file>
@@ -789,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +876,7 @@
       </c>
       <c r="I7" s="46">
         <f>SUM(D:D)</f>
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M7" s="18"/>
     </row>
@@ -944,7 +947,7 @@
       </c>
       <c r="I11" s="49">
         <f ca="1">((I5-I7)/_xlfn.DAYS(I9, NOW())) *7</f>
-        <v>8.7083333333333339</v>
+        <v>9.0125000000000011</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -1997,8 +2000,12 @@
       <c r="C84" s="27">
         <v>42695</v>
       </c>
-      <c r="D84" s="35"/>
-      <c r="E84" s="23"/>
+      <c r="D84" s="35">
+        <v>3</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="F84" s="23"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ihan kaikkea ei voi pieni ihminen ymmärtää.
</commit_message>
<xml_diff>
--- a/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
+++ b/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="36">
   <si>
     <t>Viikko</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Junction Hackathon oli tänä viikonloppuna. Sain paljon uutta oppia lohkoketjuista ja Ethereum-älykkäistä sopimuksista</t>
+  </si>
+  <si>
+    <t>Pystytin truffel-testiympäristön. Koodasin testejä ja testasin sopimusta.</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +882,7 @@
       </c>
       <c r="I7" s="46">
         <f>SUM(D:D)</f>
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="M7" s="18"/>
     </row>
@@ -950,7 +953,7 @@
       </c>
       <c r="I11" s="49">
         <f ca="1">((I5-I7)/_xlfn.DAYS(I9, NOW())) *7</f>
-        <v>9.6551724137931032</v>
+        <v>9.1241379310344826</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -2187,7 +2190,7 @@
       <c r="E98" s="23"/>
       <c r="F98" s="23"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
       <c r="B99" s="4" t="s">
         <v>7</v>
@@ -2195,8 +2198,12 @@
       <c r="C99" s="28">
         <v>42710</v>
       </c>
-      <c r="D99" s="17"/>
-      <c r="E99" s="20"/>
+      <c r="D99" s="17">
+        <v>11</v>
+      </c>
+      <c r="E99" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="F99" s="20"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pystyy vaihtamaan tiliä jolla kutsutaan funktioita.
</commit_message>
<xml_diff>
--- a/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
+++ b/Dokumentaatio/lm_lohkoketju_seurantalomake.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larty\gitrepo\ClassicCarChain\Dokumentaatio\"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="43">
   <si>
     <t>Viikko</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Muuttujien kutsu sopimuksesta</t>
+  </si>
+  <si>
+    <t>Ohjelmistoarkkitehtuuri</t>
   </si>
 </sst>
 </file>
@@ -816,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +903,7 @@
       </c>
       <c r="I7" s="46">
         <f>SUM(D:D)</f>
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M7" s="18"/>
     </row>
@@ -971,7 +974,7 @@
       </c>
       <c r="I11" s="49">
         <f ca="1">((I5-I7)/_xlfn.DAYS(I9, NOW())) *7</f>
-        <v>9.1626016260162597</v>
+        <v>9.1355932203389827</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -2532,8 +2535,12 @@
       <c r="C122" s="28">
         <v>42733</v>
       </c>
-      <c r="D122" s="17"/>
-      <c r="E122" s="20"/>
+      <c r="D122" s="17">
+        <v>4</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,8 +2551,12 @@
       <c r="C123" s="28">
         <v>42734</v>
       </c>
-      <c r="D123" s="17"/>
-      <c r="E123" s="5"/>
+      <c r="D123" s="17">
+        <v>3</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>